<commit_message>
fix excel file directory
</commit_message>
<xml_diff>
--- a/Export Data.xlsx
+++ b/Export Data.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>c--&gt;d--&gt;c</t>
+          <t>a--&gt;b</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -485,21 +485,21 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>1000000000</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>c,d</t>
+          <t>a,b</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>4,4,4</t>
+          <t>1,1,1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>c,d</t>
+          <t>a,b</t>
         </is>
       </c>
     </row>
@@ -509,7 +509,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>c--&gt;d--&gt;c</t>
+          <t>a--&gt;b</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -518,21 +518,21 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>1000000000</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>c,d</t>
+          <t>a,b</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>4,4,4</t>
+          <t>1,1,1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>c,d</t>
+          <t>a,b</t>
         </is>
       </c>
     </row>
@@ -542,7 +542,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>c--&gt;d--&gt;c</t>
+          <t>a--&gt;b</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -551,21 +551,21 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>1000000000</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>c,d</t>
+          <t>a,b</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>4,4,4</t>
+          <t>1,1,1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>c,d</t>
+          <t>a,b</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some float error
</commit_message>
<xml_diff>
--- a/Export Data.xlsx
+++ b/Export Data.xlsx
@@ -608,7 +608,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>13.6,26,31.73</t>
+          <t>14.9,31,34.76</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -641,7 +641,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -659,7 +659,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>13.1,27,30.56</t>
+          <t>14.4,31,33.59</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -674,7 +674,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -707,7 +707,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -725,12 +725,12 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>12.6,18,29.4</t>
+          <t>13.8,22,32.19</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>KMITL (Start),Suvarnabhumi Airport</t>
+          <t>KMITL (Start),Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -773,7 +773,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -791,7 +791,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>18.4,32,42.92</t>
+          <t>20.2,38,47.12</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -806,7 +806,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>25.1,45,58.56</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -872,7 +872,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -890,12 +890,12 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>18.8,31,43.86</t>
+          <t>14.9,31,34.76</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -905,7 +905,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -923,12 +923,12 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>13.1,27,30.56</t>
+          <t>20.2,38,47.12</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -956,7 +956,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1022,7 +1022,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>59.012,73,114.76</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1055,7 +1055,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>57.212,69,110.56</t>
+          <t>58.512,73,113.59</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1088,7 +1088,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>64.112,85,126.66</t>
+          <t>65.412,89,129.69</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>59.012,73,114.76</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1169,7 +1169,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1187,7 +1187,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>57.212,69,110.56</t>
+          <t>58.512,73,113.59</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>64.112,85,126.66</t>
+          <t>65.412,89,129.69</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1268,7 +1268,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1286,12 +1286,12 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>62.8,71,123.86</t>
+          <t>18.8,31,43.86</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -1334,7 +1334,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1352,12 +1352,12 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>69.3,88,139.02</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -1400,7 +1400,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1418,12 +1418,12 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>62.8,71,123.86</t>
+          <t>14.9,31,34.76</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1484,12 +1484,12 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>69.3,88,139.02</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -1532,7 +1532,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1550,7 +1550,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>59.012,73,114.76</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1583,7 +1583,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>57.212,69,110.56</t>
+          <t>58.512,73,113.59</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1598,7 +1598,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -1616,7 +1616,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>64.112,85,126.66</t>
+          <t>65.412,89,129.69</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>59.012,73,114.76</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1697,7 +1697,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -1715,7 +1715,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>57.212,69,110.56</t>
+          <t>58.512,73,113.59</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1730,7 +1730,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -1748,7 +1748,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>64.112,85,126.66</t>
+          <t>65.412,89,129.69</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -1814,12 +1814,12 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>62.912,73,123.86</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -1829,7 +1829,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
@@ -1847,12 +1847,12 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>62.512,74,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -1862,7 +1862,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -1880,12 +1880,12 @@
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -1928,7 +1928,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -1946,12 +1946,12 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>62.912,73,123.86</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -1961,7 +1961,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -1979,12 +1979,12 @@
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>62.512,74,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -1994,7 +1994,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -2012,12 +2012,12 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -2060,7 +2060,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -2078,7 +2078,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>59.012,73,114.76</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>57.212,69,110.56</t>
+          <t>58.512,73,113.59</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2126,7 +2126,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -2144,7 +2144,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>64.112,85,126.66</t>
+          <t>65.412,89,129.69</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -2192,7 +2192,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -2210,7 +2210,7 @@
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>59.012,73,114.76</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
@@ -2225,7 +2225,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -2243,7 +2243,7 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>57.212,69,110.56</t>
+          <t>58.512,73,113.59</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -2276,7 +2276,7 @@
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>64.112,85,126.66</t>
+          <t>65.412,89,129.69</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
@@ -2324,7 +2324,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
@@ -2342,12 +2342,12 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>62.912,73,123.86</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -2357,7 +2357,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -2375,12 +2375,12 @@
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>62.512,74,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -2390,7 +2390,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
@@ -2408,12 +2408,12 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -2456,7 +2456,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
@@ -2474,12 +2474,12 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>57.712,68,111.73</t>
+          <t>62.912,73,123.86</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -2489,7 +2489,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
@@ -2507,12 +2507,12 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>62.512,74,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
@@ -2540,12 +2540,12 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -2588,7 +2588,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
@@ -2606,7 +2606,7 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
@@ -2639,7 +2639,7 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
@@ -2720,7 +2720,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
@@ -2738,7 +2738,7 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -2771,7 +2771,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -2804,7 +2804,7 @@
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
@@ -2852,7 +2852,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
@@ -2870,12 +2870,12 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -2885,7 +2885,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -2903,7 +2903,7 @@
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
@@ -2936,12 +2936,12 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -2984,7 +2984,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -3002,7 +3002,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -3017,7 +3017,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -3035,7 +3035,7 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
@@ -3050,7 +3050,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
@@ -3068,12 +3068,12 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -3116,7 +3116,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
@@ -3149,7 +3149,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
@@ -3167,7 +3167,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -3182,7 +3182,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3200,7 +3200,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -3248,7 +3248,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3266,7 +3266,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
@@ -3281,7 +3281,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
@@ -3299,7 +3299,7 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -3314,7 +3314,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3332,7 +3332,7 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
@@ -3380,7 +3380,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3398,12 +3398,12 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -3413,7 +3413,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
@@ -3431,7 +3431,7 @@
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
@@ -3446,7 +3446,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
@@ -3464,12 +3464,12 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -3512,7 +3512,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
@@ -3545,7 +3545,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3563,7 +3563,7 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
@@ -3596,12 +3596,12 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -3644,7 +3644,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
@@ -3662,7 +3662,7 @@
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
@@ -3695,7 +3695,7 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3728,7 +3728,7 @@
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -3809,7 +3809,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
@@ -3827,7 +3827,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -3842,7 +3842,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3860,7 +3860,7 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G104" t="inlineStr">
@@ -3908,7 +3908,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3926,12 +3926,12 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -3941,7 +3941,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G107" t="inlineStr">
@@ -3974,7 +3974,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3992,12 +3992,12 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -4040,7 +4040,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -4058,7 +4058,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -4073,7 +4073,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -4091,7 +4091,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -4106,7 +4106,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
@@ -4124,12 +4124,12 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -4172,7 +4172,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
@@ -4190,7 +4190,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -4205,7 +4205,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -4223,7 +4223,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
@@ -4256,7 +4256,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -4304,7 +4304,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
@@ -4322,7 +4322,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -4337,7 +4337,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -4355,7 +4355,7 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>60.012,75,156.56</t>
+          <t>61.312,79,159.59</t>
         </is>
       </c>
       <c r="G119" t="inlineStr">
@@ -4370,7 +4370,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
@@ -4388,7 +4388,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>68.212,95,175.69</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -4436,7 +4436,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -4454,12 +4454,12 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -4469,7 +4469,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -4487,7 +4487,7 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G123" t="inlineStr">
@@ -4502,7 +4502,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
@@ -4520,12 +4520,12 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -4568,7 +4568,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -4586,7 +4586,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>60.512,74,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -4601,7 +4601,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4619,7 +4619,7 @@
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>65.312,80,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G127" t="inlineStr">
@@ -4634,7 +4634,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -4652,12 +4652,12 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>72.212,96,185.02</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -4700,7 +4700,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
@@ -4718,7 +4718,7 @@
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G130" t="inlineStr">
@@ -4733,7 +4733,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4751,7 +4751,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
@@ -4784,7 +4784,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -4832,7 +4832,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
@@ -4850,7 +4850,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4883,7 +4883,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
@@ -4916,7 +4916,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -4964,7 +4964,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4982,12 +4982,12 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -4997,7 +4997,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
@@ -5015,12 +5015,12 @@
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -5030,7 +5030,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -5048,12 +5048,12 @@
       </c>
       <c r="F140" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5096,7 +5096,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -5114,12 +5114,12 @@
       </c>
       <c r="F142" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5129,7 +5129,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -5147,12 +5147,12 @@
       </c>
       <c r="F143" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -5180,12 +5180,12 @@
       </c>
       <c r="F144" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -5246,7 +5246,7 @@
       </c>
       <c r="F146" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G146" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -5279,7 +5279,7 @@
       </c>
       <c r="F147" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G147" t="inlineStr">
@@ -5294,7 +5294,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -5312,7 +5312,7 @@
       </c>
       <c r="F148" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G148" t="inlineStr">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -5378,7 +5378,7 @@
       </c>
       <c r="F150" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G150" t="inlineStr">
@@ -5393,7 +5393,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -5411,7 +5411,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -5426,7 +5426,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="F152" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G152" t="inlineStr">
@@ -5492,7 +5492,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
@@ -5510,12 +5510,12 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -5543,12 +5543,12 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -5558,7 +5558,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
@@ -5576,12 +5576,12 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
@@ -5642,12 +5642,12 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5657,7 +5657,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -5675,12 +5675,12 @@
       </c>
       <c r="F159" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -5690,7 +5690,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
@@ -5708,12 +5708,12 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -5756,7 +5756,7 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
@@ -5774,7 +5774,7 @@
       </c>
       <c r="F162" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G162" t="inlineStr">
@@ -5789,7 +5789,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -5807,7 +5807,7 @@
       </c>
       <c r="F163" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G163" t="inlineStr">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
@@ -5840,7 +5840,7 @@
       </c>
       <c r="F164" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G164" t="inlineStr">
@@ -5888,7 +5888,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -5939,7 +5939,7 @@
       </c>
       <c r="F167" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G167" t="inlineStr">
@@ -5954,7 +5954,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -5972,7 +5972,7 @@
       </c>
       <c r="F168" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G168" t="inlineStr">
@@ -6020,7 +6020,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
@@ -6038,12 +6038,12 @@
       </c>
       <c r="F170" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6053,7 +6053,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -6071,12 +6071,12 @@
       </c>
       <c r="F171" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -6086,7 +6086,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -6104,12 +6104,12 @@
       </c>
       <c r="F172" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6152,7 +6152,7 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
@@ -6170,12 +6170,12 @@
       </c>
       <c r="F174" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6185,7 +6185,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -6203,12 +6203,12 @@
       </c>
       <c r="F175" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -6218,7 +6218,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
@@ -6236,12 +6236,12 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6284,7 +6284,7 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
@@ -6302,7 +6302,7 @@
       </c>
       <c r="F178" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G178" t="inlineStr">
@@ -6317,7 +6317,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -6335,7 +6335,7 @@
       </c>
       <c r="F179" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G179" t="inlineStr">
@@ -6350,7 +6350,7 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
@@ -6368,7 +6368,7 @@
       </c>
       <c r="F180" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G180" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
@@ -6434,7 +6434,7 @@
       </c>
       <c r="F182" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>61.012,99,114.76</t>
         </is>
       </c>
       <c r="G182" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -6467,7 +6467,7 @@
       </c>
       <c r="F183" t="inlineStr">
         <is>
-          <t>59.212,95,110.56</t>
+          <t>60.512,99,113.59</t>
         </is>
       </c>
       <c r="G183" t="inlineStr">
@@ -6482,7 +6482,7 @@
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
@@ -6500,7 +6500,7 @@
       </c>
       <c r="F184" t="inlineStr">
         <is>
-          <t>66.112,111,126.66</t>
+          <t>67.412,115,129.69</t>
         </is>
       </c>
       <c r="G184" t="inlineStr">
@@ -6548,7 +6548,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -6566,12 +6566,12 @@
       </c>
       <c r="F186" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6581,7 +6581,7 @@
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
@@ -6599,12 +6599,12 @@
       </c>
       <c r="F187" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -6614,7 +6614,7 @@
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
@@ -6632,12 +6632,12 @@
       </c>
       <c r="F188" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6680,7 +6680,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
@@ -6698,12 +6698,12 @@
       </c>
       <c r="F190" t="inlineStr">
         <is>
-          <t>59.712,94,111.73</t>
+          <t>64.912,99,123.86</t>
         </is>
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6713,7 +6713,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
@@ -6731,12 +6731,12 @@
       </c>
       <c r="F191" t="inlineStr">
         <is>
-          <t>64.512,100,122.92</t>
+          <t>64.2,78,127.12</t>
         </is>
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -6746,7 +6746,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -6764,12 +6764,12 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>20,43,46.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -6812,7 +6812,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -6830,7 +6830,7 @@
       </c>
       <c r="F194" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G194" t="inlineStr">
@@ -6845,7 +6845,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
@@ -6863,7 +6863,7 @@
       </c>
       <c r="F195" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G195" t="inlineStr">
@@ -6878,7 +6878,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
@@ -6896,7 +6896,7 @@
       </c>
       <c r="F196" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G196" t="inlineStr">
@@ -6944,7 +6944,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
@@ -6962,7 +6962,7 @@
       </c>
       <c r="F198" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G198" t="inlineStr">
@@ -6977,7 +6977,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -6995,7 +6995,7 @@
       </c>
       <c r="F199" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G199" t="inlineStr">
@@ -7010,7 +7010,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
@@ -7028,7 +7028,7 @@
       </c>
       <c r="F200" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G200" t="inlineStr">
@@ -7076,7 +7076,7 @@
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
@@ -7094,12 +7094,12 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7109,7 +7109,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -7127,12 +7127,12 @@
       </c>
       <c r="F203" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7142,7 +7142,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
@@ -7160,12 +7160,12 @@
       </c>
       <c r="F204" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -7208,7 +7208,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
@@ -7226,12 +7226,12 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7241,7 +7241,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -7259,12 +7259,12 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7274,7 +7274,7 @@
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
@@ -7292,12 +7292,12 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -7340,7 +7340,7 @@
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
@@ -7358,7 +7358,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
@@ -7373,7 +7373,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
@@ -7391,7 +7391,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -7406,7 +7406,7 @@
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
@@ -7424,7 +7424,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -7472,7 +7472,7 @@
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
@@ -7490,7 +7490,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -7505,7 +7505,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -7523,7 +7523,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -7538,7 +7538,7 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
@@ -7556,7 +7556,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -7604,7 +7604,7 @@
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
@@ -7622,12 +7622,12 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7637,7 +7637,7 @@
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
@@ -7655,12 +7655,12 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7670,7 +7670,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -7688,12 +7688,12 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -7736,7 +7736,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -7754,12 +7754,12 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7769,7 +7769,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
@@ -7787,12 +7787,12 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -7802,7 +7802,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
@@ -7820,12 +7820,12 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -7868,7 +7868,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
@@ -7886,7 +7886,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -7901,7 +7901,7 @@
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
@@ -7919,7 +7919,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -7934,7 +7934,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
@@ -7952,7 +7952,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -8000,7 +8000,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
@@ -8018,7 +8018,7 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -8033,7 +8033,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
@@ -8051,7 +8051,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -8066,7 +8066,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
@@ -8084,7 +8084,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -8132,7 +8132,7 @@
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
@@ -8150,12 +8150,12 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8165,7 +8165,7 @@
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
@@ -8183,12 +8183,12 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8198,7 +8198,7 @@
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
@@ -8216,12 +8216,12 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -8264,7 +8264,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
@@ -8282,12 +8282,12 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8297,7 +8297,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
@@ -8315,12 +8315,12 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8330,7 +8330,7 @@
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
@@ -8348,12 +8348,12 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -8396,7 +8396,7 @@
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
@@ -8414,7 +8414,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -8429,7 +8429,7 @@
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
@@ -8447,7 +8447,7 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -8462,7 +8462,7 @@
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
@@ -8480,7 +8480,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -8528,7 +8528,7 @@
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
@@ -8546,7 +8546,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>63.812,105,160.76</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -8561,7 +8561,7 @@
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
@@ -8579,7 +8579,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>62.012,101,156.56</t>
+          <t>63.312,105,159.59</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -8594,7 +8594,7 @@
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
@@ -8612,7 +8612,7 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>68.912,117,172.66</t>
+          <t>70.212,121,175.69</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
@@ -8660,7 +8660,7 @@
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
@@ -8678,12 +8678,12 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>67.612,86,174.29</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8693,7 +8693,7 @@
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
@@ -8711,12 +8711,12 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8726,7 +8726,7 @@
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
@@ -8744,12 +8744,12 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -8792,7 +8792,7 @@
       </c>
       <c r="B254" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C254" t="inlineStr">
@@ -8810,12 +8810,12 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>62.512,100,157.73</t>
+          <t>61.812,79,160.76</t>
         </is>
       </c>
       <c r="G254" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8825,7 +8825,7 @@
       </c>
       <c r="B255" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C255" t="inlineStr">
@@ -8843,12 +8843,12 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>67.312,106,168.92</t>
+          <t>67.112,86,173.12</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
         <is>
-          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -8858,7 +8858,7 @@
       </c>
       <c r="B256" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C256" t="inlineStr">
@@ -8876,12 +8876,12 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>66.912,91,172.66</t>
+          <t>21.3,47,49.69</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
         </is>
       </c>
     </row>
@@ -17768,7 +17768,7 @@
       </c>
       <c r="B526" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C526" t="inlineStr">
@@ -17786,12 +17786,12 @@
       </c>
       <c r="F526" t="inlineStr">
         <is>
-          <t>20,42,46.66</t>
+          <t>25.3,48,59.02</t>
         </is>
       </c>
       <c r="G526" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport</t>
         </is>
       </c>
     </row>
@@ -18164,7 +18164,7 @@
       </c>
       <c r="B538" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C538" t="inlineStr">
@@ -18182,12 +18182,12 @@
       </c>
       <c r="F538" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>69.3,88,139.02</t>
         </is>
       </c>
       <c r="G538" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -18296,7 +18296,7 @@
       </c>
       <c r="B542" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C542" t="inlineStr">
@@ -18314,12 +18314,12 @@
       </c>
       <c r="F542" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>69.3,88,139.02</t>
         </is>
       </c>
       <c r="G542" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai</t>
         </is>
       </c>
     </row>
@@ -18692,7 +18692,7 @@
       </c>
       <c r="B554" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C554" t="inlineStr">
@@ -18710,12 +18710,12 @@
       </c>
       <c r="F554" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G554" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -18824,7 +18824,7 @@
       </c>
       <c r="B558" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C558" t="inlineStr">
@@ -18842,12 +18842,12 @@
       </c>
       <c r="F558" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G558" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -19220,7 +19220,7 @@
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C570" t="inlineStr">
@@ -19238,12 +19238,12 @@
       </c>
       <c r="F570" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G570" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -19352,7 +19352,7 @@
       </c>
       <c r="B574" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C574" t="inlineStr">
@@ -19370,12 +19370,12 @@
       </c>
       <c r="F574" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>69.412,90,139.02</t>
         </is>
       </c>
       <c r="G574" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai</t>
         </is>
       </c>
     </row>
@@ -19748,7 +19748,7 @@
       </c>
       <c r="B586" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C586" t="inlineStr">
@@ -19766,12 +19766,12 @@
       </c>
       <c r="F586" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G586" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -19880,7 +19880,7 @@
       </c>
       <c r="B590" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C590" t="inlineStr">
@@ -19898,12 +19898,12 @@
       </c>
       <c r="F590" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G590" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -20276,7 +20276,7 @@
       </c>
       <c r="B602" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C602" t="inlineStr">
@@ -20294,12 +20294,12 @@
       </c>
       <c r="F602" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G602" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -20408,7 +20408,7 @@
       </c>
       <c r="B606" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C606" t="inlineStr">
@@ -20426,12 +20426,12 @@
       </c>
       <c r="F606" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G606" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -20804,7 +20804,7 @@
       </c>
       <c r="B618" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C618" t="inlineStr">
@@ -20822,12 +20822,12 @@
       </c>
       <c r="F618" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G618" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -20936,7 +20936,7 @@
       </c>
       <c r="B622" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C622" t="inlineStr">
@@ -20954,12 +20954,12 @@
       </c>
       <c r="F622" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G622" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -21332,7 +21332,7 @@
       </c>
       <c r="B634" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C634" t="inlineStr">
@@ -21350,12 +21350,12 @@
       </c>
       <c r="F634" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G634" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -21464,7 +21464,7 @@
       </c>
       <c r="B638" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C638" t="inlineStr">
@@ -21482,12 +21482,12 @@
       </c>
       <c r="F638" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>72.212,96,185.02</t>
         </is>
       </c>
       <c r="G638" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam</t>
         </is>
       </c>
     </row>
@@ -21860,7 +21860,7 @@
       </c>
       <c r="B650" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C650" t="inlineStr">
@@ -21878,12 +21878,12 @@
       </c>
       <c r="F650" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G650" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -21992,7 +21992,7 @@
       </c>
       <c r="B654" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C654" t="inlineStr">
@@ -22010,12 +22010,12 @@
       </c>
       <c r="F654" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G654" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -22388,7 +22388,7 @@
       </c>
       <c r="B666" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C666" t="inlineStr">
@@ -22406,12 +22406,12 @@
       </c>
       <c r="F666" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G666" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -22520,7 +22520,7 @@
       </c>
       <c r="B670" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C670" t="inlineStr">
@@ -22538,12 +22538,12 @@
       </c>
       <c r="F670" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G670" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -22916,7 +22916,7 @@
       </c>
       <c r="B682" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C682" t="inlineStr">
@@ -22934,12 +22934,12 @@
       </c>
       <c r="F682" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G682" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -23048,7 +23048,7 @@
       </c>
       <c r="B686" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C686" t="inlineStr">
@@ -23066,12 +23066,12 @@
       </c>
       <c r="F686" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G686" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -23444,7 +23444,7 @@
       </c>
       <c r="B698" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C698" t="inlineStr">
@@ -23462,12 +23462,12 @@
       </c>
       <c r="F698" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G698" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -23576,7 +23576,7 @@
       </c>
       <c r="B702" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C702" t="inlineStr">
@@ -23594,12 +23594,12 @@
       </c>
       <c r="F702" t="inlineStr">
         <is>
-          <t>66.112,110,126.66</t>
+          <t>71.412,116,139.02</t>
         </is>
       </c>
       <c r="G702" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,Victory monument</t>
         </is>
       </c>
     </row>
@@ -23972,7 +23972,7 @@
       </c>
       <c r="B714" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C714" t="inlineStr">
@@ -23990,12 +23990,12 @@
       </c>
       <c r="F714" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G714" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -24104,7 +24104,7 @@
       </c>
       <c r="B718" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C718" t="inlineStr">
@@ -24122,12 +24122,12 @@
       </c>
       <c r="F718" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G718" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -24500,7 +24500,7 @@
       </c>
       <c r="B730" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C730" t="inlineStr">
@@ -24518,12 +24518,12 @@
       </c>
       <c r="F730" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G730" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -24632,7 +24632,7 @@
       </c>
       <c r="B734" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C734" t="inlineStr">
@@ -24650,12 +24650,12 @@
       </c>
       <c r="F734" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G734" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -25028,7 +25028,7 @@
       </c>
       <c r="B746" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C746" t="inlineStr">
@@ -25046,12 +25046,12 @@
       </c>
       <c r="F746" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G746" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -25160,7 +25160,7 @@
       </c>
       <c r="B750" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C750" t="inlineStr">
@@ -25178,12 +25178,12 @@
       </c>
       <c r="F750" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G750" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -25556,7 +25556,7 @@
       </c>
       <c r="B762" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C762" t="inlineStr">
@@ -25574,12 +25574,12 @@
       </c>
       <c r="F762" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G762" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>
@@ -25688,7 +25688,7 @@
       </c>
       <c r="B766" t="inlineStr">
         <is>
-          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;KMITL (Start)</t>
+          <t>KMITL (Start)--&gt;Airport Rail Link Lat Krabang--&gt;Robinson Lat Krabang--&gt;Airport Rail Link Lat Krabang--&gt;Airport Rail Link Phayathai--&gt;BTS Phayathai--&gt;BTS Siam--&gt;BTS Phayathai--&gt;Victory monument--&gt;BTS Phayathai--&gt;Airport Rail Link Phayathai--&gt;Airport Rail Link Lat Krabang--&gt;The Paseo Mall Lat Krabang--&gt;Suvarnabhumi Airport--&gt;KMITL (Start)</t>
         </is>
       </c>
       <c r="C766" t="inlineStr">
@@ -25706,12 +25706,12 @@
       </c>
       <c r="F766" t="inlineStr">
         <is>
-          <t>68.912,116,172.66</t>
+          <t>74.212,122,185.02</t>
         </is>
       </c>
       <c r="G766" t="inlineStr">
         <is>
-          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
+          <t>KMITL (Start),Robinson Lat Krabang,The Paseo Mall Lat Krabang,Airport Rail Link Lat Krabang,Suvarnabhumi Airport,Airport Rail Link Phayathai,BTS Phayathai,BTS Siam,Victory monument</t>
         </is>
       </c>
     </row>

</xml_diff>